<commit_message>
Update PM04 Tidsregistrering for Toke.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM04 Tidsregistrering for Toke.xlsx
+++ b/08 Project Management/Tidsregistrering/PM04 Tidsregistrering for Toke.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Tidsregistrering af Toke</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t xml:space="preserve">Use Case Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikation med Anders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grundopsætning af rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrikker – bilag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review risikoanalyse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrikker – rapport</t>
   </si>
   <si>
     <t xml:space="preserve">Roller!</t>
@@ -529,9 +547,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>245160</xdr:colOff>
+      <xdr:colOff>244800</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -541,7 +559,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12440160" y="2517480"/>
-          <a:ext cx="184320" cy="248400"/>
+          <a:ext cx="183960" cy="248040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -571,10 +589,10 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="53.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.44"/>
@@ -715,75 +733,141 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="15"/>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.354166666666667</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.395833333333333</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="18" t="n">
         <f aca="false">E7-D7</f>
-        <v>0</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="H7" s="19" t="n">
         <f aca="false">SUM(G$3:G7)</f>
-        <v>0.3125</v>
+        <v>0.354166666666667</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="15"/>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="18" t="n">
         <f aca="false">E8-D8</f>
-        <v>0</v>
+        <v>0.0625</v>
       </c>
       <c r="H8" s="19" t="n">
         <f aca="false">SUM(G$3:G8)</f>
-        <v>0.3125</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="15"/>
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
       <c r="F9" s="20"/>
       <c r="G9" s="18" t="n">
         <f aca="false">E9-D9</f>
-        <v>0</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="H9" s="19" t="n">
         <f aca="false">SUM(G$3:G9)</f>
-        <v>0.3125</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="15"/>
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.583333333333333</v>
+      </c>
       <c r="F10" s="20"/>
       <c r="G10" s="18" t="n">
         <f aca="false">E10-D10</f>
-        <v>0</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="H10" s="19" t="n">
         <f aca="false">SUM(G$3:G10)</f>
-        <v>0.3125</v>
+        <v>0.541666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="15"/>
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0.583333333333333</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.677083333333333</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="18" t="n">
         <f aca="false">E11-D11</f>
-        <v>0</v>
+        <v>0.09375</v>
       </c>
       <c r="H11" s="19" t="n">
         <f aca="false">SUM(G$3:G11)</f>
-        <v>0.3125</v>
+        <v>0.635416666666667</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="15"/>
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="15" t="n">
+        <v>43963</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.677083333333333</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0.71875</v>
+      </c>
       <c r="F12" s="20"/>
       <c r="G12" s="18" t="n">
         <f aca="false">E12-D12</f>
-        <v>0</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="H12" s="19" t="n">
         <f aca="false">SUM(G$3:G12)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,7 +879,7 @@
       </c>
       <c r="H13" s="19" t="n">
         <f aca="false">SUM(G$3:G13)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,7 +891,7 @@
       </c>
       <c r="H14" s="19" t="n">
         <f aca="false">SUM(G$3:G14)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +903,7 @@
       </c>
       <c r="H15" s="19" t="n">
         <f aca="false">SUM(G$3:G15)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +915,7 @@
       </c>
       <c r="H16" s="19" t="n">
         <f aca="false">SUM(G$3:G16)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,7 +927,7 @@
       </c>
       <c r="H17" s="19" t="n">
         <f aca="false">SUM(G$3:G17)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,7 +939,7 @@
       </c>
       <c r="H18" s="19" t="n">
         <f aca="false">SUM(G$3:G18)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,7 +951,7 @@
       </c>
       <c r="H19" s="19" t="n">
         <f aca="false">SUM(G$3:G19)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +963,7 @@
       </c>
       <c r="H20" s="19" t="n">
         <f aca="false">SUM(G$3:G20)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +975,7 @@
       </c>
       <c r="H21" s="19" t="n">
         <f aca="false">SUM(G$3:G21)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +987,7 @@
       </c>
       <c r="H22" s="19" t="n">
         <f aca="false">SUM(G$3:G22)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +999,7 @@
       </c>
       <c r="H23" s="19" t="n">
         <f aca="false">SUM(G$3:G23)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,7 +1011,7 @@
       </c>
       <c r="H24" s="19" t="n">
         <f aca="false">SUM(G$3:G24)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +1022,7 @@
       </c>
       <c r="H25" s="19" t="n">
         <f aca="false">SUM(G$3:G25)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +1033,7 @@
       </c>
       <c r="H26" s="19" t="n">
         <f aca="false">SUM(G$3:G26)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,7 +1044,7 @@
       </c>
       <c r="H27" s="19" t="n">
         <f aca="false">SUM(G$3:G27)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,7 +1055,7 @@
       </c>
       <c r="H28" s="19" t="n">
         <f aca="false">SUM(G$3:G28)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +1066,7 @@
       </c>
       <c r="H29" s="19" t="n">
         <f aca="false">SUM(G$3:G29)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,7 +1077,7 @@
       </c>
       <c r="H30" s="19" t="n">
         <f aca="false">SUM(G$3:G30)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1088,7 @@
       </c>
       <c r="H31" s="19" t="n">
         <f aca="false">SUM(G$3:G31)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1099,7 @@
       </c>
       <c r="H32" s="19" t="n">
         <f aca="false">SUM(G$3:G32)</f>
-        <v>0.3125</v>
+        <v>0.677083333333334</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,14 +1191,14 @@
       <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1123,10 +1207,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1234,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1250,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,7 +1258,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,7 +1266,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1290,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1314,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1322,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1330,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,7 +1338,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1346,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1354,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1362,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,7 +1378,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,7 +1386,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,7 +1394,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,7 +1418,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1434,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,7 +1442,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>